<commit_message>
Se cambio el formato de la Planilla de Seguimientro a PDF
</commit_message>
<xml_diff>
--- a/web/resources/uploads/planilla_seguimiento_semestral.xlsx
+++ b/web/resources/uploads/planilla_seguimiento_semestral.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tincho\Projects\orion\web\resources\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\orion\web\resources\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68743952-EC91-4018-A005-8AC628F7375F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D771030-5FAE-4ED3-B5A1-0B12A66D25A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pla. Seg." sheetId="27" r:id="rId1"/>
@@ -33,12 +33,12 @@
     <definedName name="MEICOD_200">#REF!</definedName>
     <definedName name="PRIMERO">#REF!</definedName>
     <definedName name="PRIMERO_1">#REF!</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Pla. Seg.'!$1:$10</definedName>
     <definedName name="QUINTO">#REF!</definedName>
     <definedName name="SEGUNDO">#REF!</definedName>
     <definedName name="SEMESTRE">#REF!</definedName>
     <definedName name="SEXTO">#REF!</definedName>
     <definedName name="TERCERO">#REF!</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Pla. Seg.'!$1:$10</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
   <si>
     <t>APELLIDOS Y NOMBRES</t>
   </si>
@@ -98,10 +98,6 @@
   <si>
     <t>Prueba
 Recuperación</t>
-  </si>
-  <si>
-    <t>PUNTAJE
-FINAL</t>
   </si>
   <si>
     <t>OBSERVACIONES</t>
@@ -273,7 +269,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,12 +288,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -470,7 +460,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -481,10 +471,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -507,17 +493,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -528,10 +503,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -585,20 +556,12 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -689,38 +652,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -781,10 +712,6 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -805,6 +732,10 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -841,8 +772,46 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -870,7 +839,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1191,229 +1160,216 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Hoja12"/>
-  <dimension ref="A1:Q29"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5546875" style="3" customWidth="1"/>
-    <col min="4" max="5" width="7.44140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" style="3" customWidth="1"/>
+    <col min="4" max="5" width="7.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" style="3" customWidth="1"/>
     <col min="7" max="7" width="11" style="3" customWidth="1"/>
     <col min="8" max="8" width="12" style="3" customWidth="1"/>
-    <col min="9" max="9" width="7.88671875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="11.21875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="7.88671875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="11.44140625" style="3"/>
+    <col min="9" max="9" width="7.85546875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="36"/>
+    </row>
+    <row r="2" spans="1:11" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="39"/>
+    </row>
+    <row r="3" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="43"/>
-    </row>
-    <row r="2" spans="1:12" ht="6.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="44"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="46"/>
-    </row>
-    <row r="3" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="47" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="42"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="9"/>
+    </row>
+    <row r="5" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="49"/>
-    </row>
-    <row r="4" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="10"/>
-    </row>
-    <row r="5" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="50" t="s">
+      <c r="B5" s="44"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="88" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="88"/>
+      <c r="F5" s="89" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="89"/>
+      <c r="H5" s="89"/>
+      <c r="I5" s="89"/>
+      <c r="J5" s="83" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="84" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="46"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="90" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="90"/>
+      <c r="F6" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="59" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="60"/>
-      <c r="F5" s="61" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" s="63" t="s">
+      <c r="G6" s="91"/>
+      <c r="H6" s="91"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="85" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="L5" s="64"/>
-    </row>
-    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="53"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="65" t="s">
+    </row>
+    <row r="7" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="49"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="90" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="90"/>
+      <c r="F7" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="66"/>
-      <c r="F6" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="K6" s="35" t="s">
+      <c r="G7" s="91"/>
+      <c r="H7" s="91"/>
+      <c r="I7" s="91"/>
+      <c r="J7" s="87" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="36"/>
-    </row>
-    <row r="7" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="56"/>
-      <c r="B7" s="57"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="65" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="66"/>
-      <c r="F7" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K7" s="4" t="s">
+    </row>
+    <row r="8" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="11"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="67" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="78"/>
+      <c r="J9" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="52" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="57"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="79"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="53"/>
+    </row>
+    <row r="11" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>-1</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="L7" s="13"/>
-    </row>
-    <row r="8" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="15"/>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="71" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="83" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="67" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="69" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="69" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="69" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="67" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="83" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="93"/>
-      <c r="J9" s="69" t="s">
-        <v>15</v>
-      </c>
-      <c r="K9" s="67" t="s">
-        <v>16</v>
-      </c>
-      <c r="L9" s="67" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="72"/>
-      <c r="B10" s="84"/>
-      <c r="C10" s="68"/>
-      <c r="D10" s="70"/>
-      <c r="E10" s="70"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="84"/>
-      <c r="I10" s="94"/>
-      <c r="J10" s="70"/>
-      <c r="K10" s="68"/>
-      <c r="L10" s="68"/>
-    </row>
-    <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="16">
-        <v>-1</v>
-      </c>
-      <c r="B11" s="16" t="s">
+      <c r="C11" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="D11" s="1">
         <v>-12</v>
@@ -1424,285 +1380,269 @@
       <c r="F11" s="1">
         <v>-32</v>
       </c>
-      <c r="G11" s="26">
+      <c r="G11" s="21">
         <v>-50</v>
       </c>
-      <c r="H11" s="91" t="s">
-        <v>45</v>
-      </c>
-      <c r="I11" s="92"/>
-      <c r="J11" s="17">
+      <c r="H11" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11" s="77"/>
+      <c r="J11" s="4">
         <v>-51</v>
       </c>
-      <c r="K11" s="17"/>
-      <c r="L11" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="37" t="s">
+      <c r="K11" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="31"/>
+      <c r="C13" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="79" t="s">
+      <c r="D13" s="64"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="28">
+        <v>-100</v>
+      </c>
+      <c r="G13" s="29"/>
+      <c r="H13" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="59"/>
+      <c r="J13" s="60"/>
+      <c r="K13" s="15"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="79"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="34">
-        <v>-100</v>
-      </c>
-      <c r="G13" s="97"/>
-      <c r="H13" s="73" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="74"/>
-      <c r="J13" s="75"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="39" t="s">
+      <c r="B14" s="33"/>
+      <c r="C14" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="40"/>
-      <c r="C14" s="76" t="s">
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="28">
+        <v>-101</v>
+      </c>
+      <c r="G14" s="29"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="15"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="34">
-        <v>-101</v>
-      </c>
-      <c r="G14" s="97"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="78"/>
-      <c r="J14" s="78"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="21"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="79" t="s">
+      <c r="D15" s="64"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="28">
+        <v>-102</v>
+      </c>
+      <c r="G15" s="29"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="15"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="79"/>
-      <c r="E15" s="80"/>
-      <c r="F15" s="34">
-        <v>-102</v>
-      </c>
-      <c r="G15" s="97"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="78"/>
-      <c r="J15" s="78"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="21"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="80" t="s">
+      <c r="D16" s="66"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="28">
+        <v>-103</v>
+      </c>
+      <c r="G16" s="29"/>
+      <c r="H16" s="63"/>
+      <c r="I16" s="63"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="17"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="81"/>
-      <c r="E16" s="81"/>
-      <c r="F16" s="34">
-        <v>-103</v>
-      </c>
-      <c r="G16" s="97"/>
-      <c r="H16" s="78"/>
-      <c r="I16" s="78"/>
-      <c r="J16" s="78"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="79" t="s">
+      <c r="D17" s="64"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="28">
+        <v>-104</v>
+      </c>
+      <c r="G17" s="29"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="17"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="79"/>
-      <c r="E17" s="80"/>
-      <c r="F17" s="34">
-        <v>-104</v>
-      </c>
-      <c r="G17" s="97"/>
-      <c r="H17" s="78"/>
-      <c r="I17" s="78"/>
-      <c r="J17" s="78"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="24" t="s">
+      <c r="D19" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="95" t="s">
+      <c r="E19" s="80"/>
+      <c r="F19" s="81"/>
+      <c r="G19" s="81"/>
+      <c r="H19" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="95"/>
-      <c r="F19" s="96"/>
-      <c r="G19" s="96"/>
-      <c r="H19" s="88" t="s">
+      <c r="I19" s="73"/>
+      <c r="J19" s="73"/>
+      <c r="K19" s="15"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="70"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="72"/>
+      <c r="H20" s="73"/>
+      <c r="I20" s="73"/>
+      <c r="J20" s="73"/>
+      <c r="K20" s="15"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="70"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="72"/>
+      <c r="H21" s="73"/>
+      <c r="I21" s="73"/>
+      <c r="J21" s="73"/>
+      <c r="K21" s="15"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="I19" s="88"/>
-      <c r="J19" s="88"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="86"/>
-      <c r="E20" s="87"/>
-      <c r="F20" s="82"/>
-      <c r="G20" s="82"/>
-      <c r="H20" s="88"/>
-      <c r="I20" s="88"/>
-      <c r="J20" s="88"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="86"/>
-      <c r="E21" s="87"/>
-      <c r="F21" s="82"/>
-      <c r="G21" s="82"/>
-      <c r="H21" s="88"/>
-      <c r="I21" s="88"/>
-      <c r="J21" s="88"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="28" t="s">
+      <c r="D22" s="70"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="74"/>
+      <c r="I22" s="74"/>
+      <c r="J22" s="74"/>
+      <c r="K22" s="8"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+    </row>
+    <row r="25" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="75" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="75"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="75"/>
+      <c r="J25" s="75"/>
+      <c r="K25" s="7"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="82" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="86"/>
-      <c r="E22" s="87"/>
-      <c r="F22" s="87"/>
-      <c r="G22" s="87"/>
-      <c r="H22" s="89"/>
-      <c r="I22" s="89"/>
-      <c r="J22" s="89"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="25"/>
-      <c r="P23" s="7"/>
-      <c r="Q23" s="7"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-    </row>
-    <row r="25" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="9"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="90" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="90"/>
-      <c r="F25" s="90"/>
-      <c r="G25" s="90"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="90"/>
-      <c r="J25" s="90"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A26" s="9"/>
-      <c r="B26" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="85" t="s">
+      <c r="E26" s="69"/>
+      <c r="F26" s="69"/>
+      <c r="G26" s="69"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="85"/>
-      <c r="F26" s="85"/>
-      <c r="G26" s="85"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="85" t="s">
-        <v>30</v>
-      </c>
-      <c r="J26" s="85"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-    </row>
-    <row r="28" spans="1:17" ht="0.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.3"/>
+      <c r="J26" s="69"/>
+      <c r="K26" s="5"/>
+    </row>
+    <row r="28" spans="1:16" ht="0.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="44">
+  <mergeCells count="41">
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="D26:G26"/>
     <mergeCell ref="I26:J26"/>
@@ -1729,19 +1669,16 @@
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="G9:G10"/>
-    <mergeCell ref="L9:L10"/>
     <mergeCell ref="K9:K10"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A1:L2"/>
-    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="A1:K2"/>
+    <mergeCell ref="A3:K3"/>
     <mergeCell ref="A5:C7"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:I5"/>
-    <mergeCell ref="K5:L5"/>
     <mergeCell ref="D6:E6"/>
-    <mergeCell ref="K6:L6"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="F7:I7"/>
     <mergeCell ref="C9:C10"/>

</xml_diff>